<commit_message>
code updated to read column values
</commit_message>
<xml_diff>
--- a/matchExcel.xlsx
+++ b/matchExcel.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\TechShelke\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\TechShelke\automate-match-service\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{812D675D-6A9C-480E-B97F-81A77D7403CF}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9EDC10B-60C4-4148-B016-94A0B8F28D1C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12375" xr2:uid="{A6BE0058-BB02-4F5C-B942-6DFD2085D2C0}"/>
   </bookViews>
@@ -30,9 +30,6 @@
     <t>ANI</t>
   </si>
   <si>
-    <t>AccountNumber</t>
-  </si>
-  <si>
     <t>Sys</t>
   </si>
   <si>
@@ -40,6 +37,9 @@
   </si>
   <si>
     <t>Agent</t>
+  </si>
+  <si>
+    <t>Account Number</t>
   </si>
 </sst>
 </file>
@@ -394,13 +394,13 @@
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -408,16 +408,16 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>3</v>
-      </c>
-      <c r="E1" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">

</xml_diff>